<commit_message>
Updated BOMfile with links
</commit_message>
<xml_diff>
--- a/hunscan_V100_DCI_BOM.xlsx
+++ b/hunscan_V100_DCI_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pollock\Documents\Repo\hardware_dev_df\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D9A9EC-015D-40BE-87FE-BB022F3E6220}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0FE8DF-3C7E-48E2-A17F-5D0858490DF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6BB6B917-AF56-4B92-AD82-C7250C129153}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{6BB6B917-AF56-4B92-AD82-C7250C129153}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
   <si>
     <t>Qty</t>
   </si>
@@ -215,13 +215,37 @@
   </si>
   <si>
     <t xml:space="preserve">HUNSCAN BOMList(V1.0.0 DCI) </t>
+  </si>
+  <si>
+    <t>150mW</t>
+  </si>
+  <si>
+    <t>Schottky Diodes &amp; Rectifiers Schottky 150mW</t>
+  </si>
+  <si>
+    <t>https://my.mouser.com/ProductDetail/Taiwan-Semiconductor/TSS0340U-RGG?qs=QEzMiVqgwc0IWpzjx4IhRg==</t>
+  </si>
+  <si>
+    <t>LQM18PH1R0MFRL</t>
+  </si>
+  <si>
+    <t>TSS0340U RGG</t>
+  </si>
+  <si>
+    <t>1uH 20% 360mA 0.25ohm</t>
+  </si>
+  <si>
+    <t>Fixed Inductors 0603 1uH 20% 360mA 0.25ohm</t>
+  </si>
+  <si>
+    <t>https://my.mouser.com/ProductDetail/Murata-Electronics/LQM18PH1R0MFRL?qs=rkhjVJ6%2F3EIdfbYqdWbcig%3D%3D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +311,12 @@
     <font>
       <sz val="7"/>
       <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -463,6 +493,17 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -472,18 +513,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -801,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99144AAD-22C5-4B4D-A92C-45347D70963E}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -819,19 +849,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="37"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="42"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -1154,9 +1184,15 @@
         <v>1</v>
       </c>
       <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="17"/>
+      <c r="E12" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>62</v>
+      </c>
       <c r="H12" s="10" t="s">
         <v>43</v>
       </c>
@@ -1166,32 +1202,42 @@
       <c r="J12" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="9"/>
-    </row>
-    <row r="13" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K12" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>11</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="35" t="s">
         <v>58</v>
       </c>
       <c r="C13" s="19">
         <v>1</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="40" t="s">
+      <c r="D13" s="36"/>
+      <c r="E13" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="41" t="s">
+      <c r="I13" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="38" t="s">
+      <c r="J13" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="K13" s="42"/>
+      <c r="K13" s="26" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
@@ -1285,8 +1331,10 @@
   <hyperlinks>
     <hyperlink ref="K10" r:id="rId1" xr:uid="{41EB3C0B-DB30-492A-A8BA-31DA07101753}"/>
     <hyperlink ref="K11" r:id="rId2" display="https://www.digikey.my/product-detail/en/molex/1050170001/WM1399CT-ND/2350885?utm_adgroup=Molex&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_EN_Supplier&amp;utm_term=&amp;productid=&amp;gclid=Cj0KCQjwirz3BRD_ARIsAImf7LN2gszsfY4YytdwDBAgQIgrsk3-NnYL0r1gYOgbd5p5W7NCgwE0Uh8aAmPcEALw_wcB" xr:uid="{88F3E175-F34E-48F2-A930-0447EE20241B}"/>
+    <hyperlink ref="K12" r:id="rId3" xr:uid="{DDA79025-8F9C-4021-B42B-0F4DBC6E3E43}"/>
+    <hyperlink ref="K13" r:id="rId4" xr:uid="{89601095-406E-43F4-94C5-C80F25D751E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOM and Gerber
</commit_message>
<xml_diff>
--- a/hunscan_V100_DCI_BOM.xlsx
+++ b/hunscan_V100_DCI_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pollock\Documents\Repo\hardware_dev_df\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0FE8DF-3C7E-48E2-A17F-5D0858490DF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D387B3A3-696D-445C-8E2A-A0B21D95E375}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{6BB6B917-AF56-4B92-AD82-C7250C129153}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6BB6B917-AF56-4B92-AD82-C7250C129153}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="70">
   <si>
     <t>Qty</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>https://my.mouser.com/ProductDetail/Murata-Electronics/LQM18PH1R0MFRL?qs=rkhjVJ6%2F3EIdfbYqdWbcig%3D%3D</t>
+  </si>
+  <si>
+    <t>R3</t>
   </si>
 </sst>
 </file>
@@ -504,6 +507,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -513,7 +517,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -829,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99144AAD-22C5-4B4D-A92C-45347D70963E}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -849,19 +852,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="42"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="43"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -1012,258 +1015,274 @@
       </c>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>48</v>
+      <c r="B7" s="13" t="s">
+        <v>69</v>
       </c>
       <c r="C7" s="8">
-        <v>2</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>39</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>33</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="K7" s="9"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C8" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>15</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" s="8"/>
+      <c r="J8" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C9" s="8">
         <v>1</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>37</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E9" s="8"/>
       <c r="F9" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>33</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>35</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C10" s="8">
         <v>1</v>
       </c>
-      <c r="D10" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>27</v>
+      <c r="D10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="K10" s="26" t="s">
-        <v>52</v>
+      <c r="J10" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>9</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>56</v>
+      <c r="B11" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="C11" s="8">
         <v>1</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" t="s">
-        <v>53</v>
+      <c r="D11" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="10"/>
+        <v>51</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="J11" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K11" s="26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>10</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>57</v>
+      <c r="B12" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="C12" s="8">
         <v>1</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>33</v>
-      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="10"/>
       <c r="J12" s="22" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="K12" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>11</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11">
+        <v>12</v>
+      </c>
+      <c r="B14" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C14" s="19">
         <v>1</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="43" t="s">
+      <c r="D14" s="36"/>
+      <c r="E14" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="43" t="s">
+      <c r="F14" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="43" t="s">
+      <c r="G14" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="37" t="s">
+      <c r="H14" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="38" t="s">
+      <c r="I14" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="35" t="s">
+      <c r="J14" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="K13" s="26" t="s">
+      <c r="K14" s="26" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="25"/>
-    </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="32"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="25"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="27"/>
@@ -1314,13 +1333,26 @@
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
       <c r="I19" s="30"/>
+      <c r="J19" s="31"/>
       <c r="K19" s="32"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K20" s="24"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="30"/>
+      <c r="K20" s="32"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+      <c r="K21" s="24"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1329,10 +1361,10 @@
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1" xr:uid="{41EB3C0B-DB30-492A-A8BA-31DA07101753}"/>
-    <hyperlink ref="K11" r:id="rId2" display="https://www.digikey.my/product-detail/en/molex/1050170001/WM1399CT-ND/2350885?utm_adgroup=Molex&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_EN_Supplier&amp;utm_term=&amp;productid=&amp;gclid=Cj0KCQjwirz3BRD_ARIsAImf7LN2gszsfY4YytdwDBAgQIgrsk3-NnYL0r1gYOgbd5p5W7NCgwE0Uh8aAmPcEALw_wcB" xr:uid="{88F3E175-F34E-48F2-A930-0447EE20241B}"/>
-    <hyperlink ref="K12" r:id="rId3" xr:uid="{DDA79025-8F9C-4021-B42B-0F4DBC6E3E43}"/>
-    <hyperlink ref="K13" r:id="rId4" xr:uid="{89601095-406E-43F4-94C5-C80F25D751E4}"/>
+    <hyperlink ref="K11" r:id="rId1" xr:uid="{41EB3C0B-DB30-492A-A8BA-31DA07101753}"/>
+    <hyperlink ref="K12" r:id="rId2" display="https://www.digikey.my/product-detail/en/molex/1050170001/WM1399CT-ND/2350885?utm_adgroup=Molex&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_EN_Supplier&amp;utm_term=&amp;productid=&amp;gclid=Cj0KCQjwirz3BRD_ARIsAImf7LN2gszsfY4YytdwDBAgQIgrsk3-NnYL0r1gYOgbd5p5W7NCgwE0Uh8aAmPcEALw_wcB" xr:uid="{88F3E175-F34E-48F2-A930-0447EE20241B}"/>
+    <hyperlink ref="K13" r:id="rId3" xr:uid="{DDA79025-8F9C-4021-B42B-0F4DBC6E3E43}"/>
+    <hyperlink ref="K14" r:id="rId4" xr:uid="{89601095-406E-43F4-94C5-C80F25D751E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>

</xml_diff>